<commit_message>
COMMENT TO DESCRIBE THE INTENTION OF THE COMMIT
</commit_message>
<xml_diff>
--- a/files/Materiallist.xlsx
+++ b/files/Materiallist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\google\UoM\Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\google\UoM\Website\OpenPnuUoM.github.io\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6FAD3C4-D956-4751-A6B6-97F16920AB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36827834-A15C-4CD2-A8DB-414DEA2E3BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="98">
   <si>
     <t>Comment</t>
   </si>
@@ -215,18 +215,12 @@
     <t xml:space="preserve">LCSC Part </t>
   </si>
   <si>
-    <t>Price($)</t>
-  </si>
-  <si>
     <t>POSITIVE PRESSURE SENSOR(0,15 psi)</t>
   </si>
   <si>
     <t>HYBRID PRESSURE SENSOR(±15 psi)</t>
   </si>
   <si>
-    <t>WIRE</t>
-  </si>
-  <si>
     <t>MICRO AIR PUMP</t>
   </si>
   <si>
@@ -236,9 +230,6 @@
     <t>3D PRINTED COMPONENTS</t>
   </si>
   <si>
-    <t>POWER</t>
-  </si>
-  <si>
     <t>6MM TUBE</t>
   </si>
   <si>
@@ -248,7 +239,82 @@
     <t>1m</t>
   </si>
   <si>
-    <t>THREE-WAY CONNECTION</t>
+    <t>T-CONNECTOR</t>
+  </si>
+  <si>
+    <t>Price per unit($)</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_1MR-1004-1_C105578.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Resistors_TY-OHM-Elec-RMC06034-7k5-N_C269694.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Crystals_Yangxing-Tech-X49SM8MSD2SC_C12674.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_YAGEO-RC0603FR-0710KL_C98220.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Tantalum-Capacitors_CEC-Shenzhen-Zhenhua-XinYun-Elec-CA45-B-25V-10uF-K_C128259.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_FH-Guangdong-Fenghua-Advanced-Tech-0603CG200J500NT_C91702.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Crystals_Yangxing-Tech-X803832768KGD4GI_C12675.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Walsin-Tech-Corp-0603B104K250CT_C83054.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Tantalum-Capacitors_Kyocera-AVX-TAJC107K010RNJ_C8649.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Tantalum-Capacitors_Kyocera-AVX-TAJC337K006RNJ_C11377.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Resistor-Today-HPCR0603F510RK9_C365184.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Push-Switches_SMK-Corp-JPM1040-2013FC_C516061.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/USB-ICs_WCH-Jiangsu-Qin-Heng-CH340C_C84681.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Schottky-Barrier-Diodes-SBD_DIYI-Elec-Tech-SS110_C85588.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Light-Emitting-Diodes-LED_MEIHUA-MHT192UBCT_C389520.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/LED-Drivers_NXP-Semicon-PCA9685PW-Q900-118_C92206.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Microcontroller-Units-MCUs-MPUs-SOCs_STMicroelectronics-STM32F103C8T6_C8734.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Motor-Driver-ICs_TOSHIBA-TB6612FNG-C-8-EL_C141517.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/I-O-Expanders_NXP-Semicon-PCA9555PW-118_C128392.html</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_Advanced-Monolithic-Systems-AMS1117-3-3_C6186.html</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Honeywell/ABPDANV015PGSA3?qs=OTrKUuiFdkZBd6HAHATCgg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Honeywell/ABPDANN015PDSA3?qs=PqoDHHvF64%2FiGr12hdg%252BZw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.skoocomtech.com/air-pump/vacuum-pump/small-size-vacuum-pump-sc3710pm.html</t>
+  </si>
+  <si>
+    <t>https://www.skoocomtech.com/air-valve/3-way-valve/quick-exhaust-valve-sc0626gf.html</t>
   </si>
 </sst>
 </file>
@@ -745,7 +811,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -769,6 +835,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -869,13 +938,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D625CD6-C2FA-4943-B437-683933A7F903}" name="Table1" displayName="Table1" ref="A2:E34" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D625CD6-C2FA-4943-B437-683933A7F903}" name="Table1" displayName="Table1" ref="A2:F32" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8ABC82C3-E01B-41CF-A268-354BCF9B9914}" name="Material for Printed circuit board (PCB)" headerRowDxfId="0"/>
     <tableColumn id="2" xr3:uid="{CF41A298-C0B7-4709-81A8-FB847062F760}" name="Column1"/>
     <tableColumn id="3" xr3:uid="{43B181DE-E4C7-42E8-9FB6-23D09D6A7B42}" name="Column2"/>
     <tableColumn id="4" xr3:uid="{0D7AEEF9-78DB-47E9-BC65-C1FD7A3DF7C4}" name="Column3" headerRowDxfId="1" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{2EAAF072-D644-479F-BDBB-C0975B430163}" name="Column4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{0D81B92B-7AE4-4916-B1CB-B11A6ABD7BFF}" name="Column5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1178,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,13 +1260,13 @@
     <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1210,10 +1280,10 @@
         <v>57</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1227,8 +1297,11 @@
       <c r="E3" s="6">
         <v>1.5E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1242,8 +1315,11 @@
       <c r="E4" s="6">
         <v>2.8999999999999998E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1257,8 +1333,11 @@
       <c r="E5" s="6">
         <v>9.4299999999999995E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1272,8 +1351,11 @@
       <c r="E6" s="6">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1287,8 +1369,11 @@
       <c r="E7" s="6">
         <v>0.1229</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1302,8 +1387,11 @@
       <c r="E8" s="6">
         <v>4.1999999999999997E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1317,8 +1405,11 @@
       <c r="E9" s="6">
         <v>0.3352</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1332,8 +1423,11 @@
       <c r="E10" s="6">
         <v>2.7000000000000001E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -1347,8 +1441,11 @@
       <c r="E11" s="6">
         <v>0.193</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
@@ -1362,8 +1459,11 @@
       <c r="E12" s="6">
         <v>0.54820000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1377,8 +1477,11 @@
       <c r="E13" s="6">
         <v>7.9000000000000008E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1392,8 +1495,11 @@
       <c r="E14" s="6">
         <v>0.31459999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
@@ -1407,8 +1513,11 @@
       <c r="E15" s="6">
         <v>0.51580000000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
@@ -1422,8 +1531,11 @@
       <c r="E16" s="6">
         <v>2.7900000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
@@ -1437,8 +1549,11 @@
       <c r="E17" s="6">
         <v>3.2599999999999997E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1452,8 +1567,11 @@
       <c r="E18" s="6">
         <v>2.3658999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -1467,8 +1585,11 @@
       <c r="E19" s="6">
         <v>3.5074000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
@@ -1482,8 +1603,11 @@
       <c r="E20" s="6">
         <v>5.1357999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
@@ -1497,8 +1621,11 @@
       <c r="E21" s="6">
         <v>1.1848000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
@@ -1512,10 +1639,13 @@
       <c r="E22" s="6">
         <v>0.16769999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>58</v>
@@ -1525,12 +1655,15 @@
         <v>5</v>
       </c>
       <c r="E23" s="6">
-        <v>103.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14.7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>59</v>
@@ -1540,14 +1673,17 @@
         <v>5</v>
       </c>
       <c r="E24" s="6">
-        <v>98.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+        <v>18.39</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>0</v>
       </c>
@@ -1561,86 +1697,86 @@
         <v>57</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="4">
+        <v>20</v>
+      </c>
+      <c r="E27" s="10">
+        <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="4">
+        <v>10</v>
+      </c>
+      <c r="E28" s="10">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="10">
         <v>60</v>
       </c>
-      <c r="D29" s="4">
-        <v>20</v>
-      </c>
-      <c r="E29" s="1">
-        <v>121.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="4">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1">
-        <v>30.4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="4">
+      <c r="D32" s="4">
         <v>10</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>